<commit_message>
Line and var type now printed
</commit_message>
<xml_diff>
--- a/HW2-3.xlsx
+++ b/HW2-3.xlsx
@@ -585,13 +585,13 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -611,13 +611,13 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -637,13 +637,13 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -715,13 +715,13 @@
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -897,13 +897,13 @@
         <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>5</v>
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -975,16 +975,16 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1053,13 +1053,13 @@
         <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1076,16 +1076,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D28" t="n">
         <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1180,6 +1180,9 @@
       <c r="G2" t="n">
         <v>2.555555555555555</v>
       </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1203,6 +1206,9 @@
       <c r="G3" t="n">
         <v>2.5</v>
       </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1226,6 +1232,9 @@
       <c r="G4" t="n">
         <v>6</v>
       </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1235,19 +1244,22 @@
         <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>4</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>2.875</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1270,7 +1282,10 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>2.5</v>
+        <v>2.333333333333333</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -1293,7 +1308,10 @@
         <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>9.272727272727273</v>
+        <v>9.090909090909092</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -1316,7 +1334,10 @@
         <v>3</v>
       </c>
       <c r="G8" t="n">
-        <v>8.857142857142858</v>
+        <v>8.642857142857142</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1339,7 +1360,10 @@
         <v>3</v>
       </c>
       <c r="G9" t="n">
-        <v>2.9375</v>
+        <v>2.75</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1362,7 +1386,10 @@
         <v>3</v>
       </c>
       <c r="G10" t="n">
-        <v>3.1875</v>
+        <v>3</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1385,7 +1412,10 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>104.4444444444444</v>
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -1408,7 +1438,10 @@
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>4</v>
+        <v>3.888888888888889</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1431,7 +1464,10 @@
         <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>2.666666666666667</v>
+        <v>2.333333333333333</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1456,6 +1492,9 @@
       <c r="G14" t="n">
         <v>2.8125</v>
       </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1477,7 +1516,10 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>4.642857142857143</v>
+        <v>4.142857142857143</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -1485,10 +1527,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -1500,7 +1542,10 @@
         <v>5</v>
       </c>
       <c r="G16" t="n">
-        <v>61.9375</v>
+        <v>6.266666666666667</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1523,7 +1568,10 @@
         <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>163.5</v>
+        <v>6</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1531,10 +1579,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -1546,7 +1594,10 @@
         <v>3</v>
       </c>
       <c r="G18" t="n">
-        <v>6.4375</v>
+        <v>5.823529411764706</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1569,7 +1620,10 @@
         <v>3</v>
       </c>
       <c r="G19" t="n">
-        <v>6.882352941176471</v>
+        <v>6.588235294117647</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1577,10 +1631,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -1592,7 +1646,10 @@
         <v>4</v>
       </c>
       <c r="G20" t="n">
-        <v>4.466666666666667</v>
+        <v>3.888888888888889</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1615,7 +1672,10 @@
         <v>3</v>
       </c>
       <c r="G21" t="n">
-        <v>6</v>
+        <v>5.769230769230769</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1623,10 +1683,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
@@ -1638,7 +1698,10 @@
         <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>4</v>
+        <v>3.833333333333333</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1646,22 +1709,25 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>2.666666666666667</v>
+        <v>2.5</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1669,22 +1735,25 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>5.5</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1707,7 +1776,10 @@
         <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>149.3333333333333</v>
+        <v>4.833333333333333</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1715,10 +1787,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1730,7 +1802,10 @@
         <v>4</v>
       </c>
       <c r="G26" t="n">
-        <v>2.266666666666667</v>
+        <v>2.0625</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1753,7 +1828,10 @@
         <v>3</v>
       </c>
       <c r="G27" t="n">
-        <v>3.5</v>
+        <v>3.4</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1761,22 +1839,25 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C28" t="n">
+        <v>9</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>6</v>
+      </c>
+      <c r="F28" t="n">
         <v>7</v>
       </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" t="n">
-        <v>5</v>
-      </c>
-      <c r="F28" t="n">
-        <v>4</v>
-      </c>
       <c r="G28" t="n">
-        <v>5.125</v>
+        <v>5.636363636363637</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaning up to branch and edit program to disregard certain vars
</commit_message>
<xml_diff>
--- a/HW2-3.xlsx
+++ b/HW2-3.xlsx
@@ -920,7 +920,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
         <v>4</v>
@@ -972,7 +972,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" t="n">
         <v>4</v>
@@ -1293,7 +1293,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
         <v>5</v>
@@ -1302,13 +1302,13 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>9.090909090909092</v>
+        <v>8.916666666666666</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
@@ -1319,7 +1319,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
@@ -1331,10 +1331,10 @@
         <v>4</v>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>8.642857142857142</v>
+        <v>9</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1363,7 +1363,7 @@
         <v>2.75</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1423,7 +1423,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
         <v>4</v>
@@ -1435,10 +1435,10 @@
         <v>4</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>3.888888888888889</v>
+        <v>4.8</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
         <v>4.142857142857143</v>
@@ -1527,7 +1527,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" t="n">
         <v>6</v>
@@ -1536,13 +1536,13 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>5</v>
       </c>
       <c r="G16" t="n">
-        <v>6.266666666666667</v>
+        <v>6</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1605,7 +1605,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" t="n">
         <v>7</v>
@@ -1620,7 +1620,7 @@
         <v>3</v>
       </c>
       <c r="G19" t="n">
-        <v>6.588235294117647</v>
+        <v>6.277777777777778</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1657,22 +1657,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C21" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>3</v>
       </c>
       <c r="G21" t="n">
-        <v>5.769230769230769</v>
+        <v>5.125</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1735,7 +1735,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" t="n">
         <v>3</v>
@@ -1744,13 +1744,13 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>6</v>
       </c>
       <c r="G24" t="n">
-        <v>5.5</v>
+        <v>5.352941176470588</v>
       </c>
       <c r="H24" t="n">
         <v>1</v>
@@ -1839,7 +1839,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C28" t="n">
         <v>9</v>
@@ -1848,13 +1848,13 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>7</v>
       </c>
       <c r="G28" t="n">
-        <v>5.636363636363637</v>
+        <v>5.434782608695652</v>
       </c>
       <c r="H28" t="n">
         <v>1</v>

</xml_diff>